<commit_message>
fix bug row index test 2 and and api spesification
</commit_message>
<xml_diff>
--- a/test2/storage/files/Type_B.xlsx
+++ b/test2/storage/files/Type_B.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\xampp\htdocs\php-assesment\test2\storage\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E875EB70-8864-40C2-8954-1EFC4202EB1F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62EFC57A-4AE9-4310-9398-2FF267DCE8E8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -388,7 +388,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -422,8 +422,7 @@
       <c r="E3" s="1"/>
     </row>
     <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
+      <c r="B4" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>